<commit_message>
Focus ends up at first column of row 6
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_DO_template.xlsx
+++ b/templates/aspace_import_excel_DO_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19065" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -757,8 +757,8 @@
   <dimension ref="A1:ALI6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>